<commit_message>
FIx ages for David Roche and Peter Douthwright
</commit_message>
<xml_diff>
--- a/data/2020-02-04/Senior Cubers Worldwide - Weekly Competition - 2020-02-04.xlsx
+++ b/data/2020-02-04/Senior Cubers Worldwide - Weekly Competition - 2020-02-04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F731F270-F987-465F-BF5C-2FBA29CF10D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4AD26C-87CB-408E-910A-12E61D7780CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -894,7 +894,7 @@
   <dimension ref="A1:L1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1598,7 +1598,7 @@
         <v>109</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="D22" s="17">
         <v>44.11</v>

</xml_diff>

<commit_message>
Patch 2020-02-04/4x4x4 to use DNS
</commit_message>
<xml_diff>
--- a/data/2020-02-04/Senior Cubers Worldwide - Weekly Competition - 2020-02-04.xlsx
+++ b/data/2020-02-04/Senior Cubers Worldwide - Weekly Competition - 2020-02-04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\scw-comp\data\2020-02-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4AD26C-87CB-408E-910A-12E61D7780CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8683ED8F-4055-433D-8197-45D4B9095555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3x3" sheetId="1" r:id="rId1"/>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>1:26.77</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>https://www.facebook.com/pete.lee.9003/videos/2505517469558727/</t>
@@ -440,6 +437,9 @@
   </si>
   <si>
     <t>Jamie Brady (Deansie)</t>
+  </si>
+  <si>
+    <t>DNS</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   </sheetPr>
   <dimension ref="A1:L1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -951,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>9</v>
@@ -1021,7 +1021,7 @@
         <v>15.65</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" s="17">
         <v>12.1</v>
@@ -1124,7 +1124,7 @@
         <v>19.2</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F8" s="21">
         <v>18.489999999999998</v>
@@ -1150,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>21</v>
@@ -1175,7 +1175,7 @@
         <v>22.86</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="12.75">
@@ -1183,7 +1183,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>21</v>
@@ -1192,7 +1192,7 @@
         <v>21.68</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="17">
         <v>21.02</v>
@@ -1210,7 +1210,7 @@
         <v>21.42</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="12.75">
@@ -1243,7 +1243,7 @@
         <v>20.170000000000002</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="12.75">
@@ -1251,7 +1251,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>16</v>
@@ -1260,7 +1260,7 @@
         <v>22.72</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" s="24">
         <v>17.3</v>
@@ -1278,7 +1278,7 @@
         <v>31.93</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="12.75">
@@ -1286,7 +1286,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>21</v>
@@ -1295,7 +1295,7 @@
         <v>23.58</v>
       </c>
       <c r="E13" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="17">
         <v>23.38</v>
@@ -1313,7 +1313,7 @@
         <v>25.9</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="12.75">
@@ -1321,7 +1321,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>16</v>
@@ -1346,7 +1346,7 @@
         <v>36.89</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="12.75">
@@ -1354,7 +1354,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>21</v>
@@ -1370,7 +1370,7 @@
         <v>24.74</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I15" s="17">
         <v>22.48</v>
@@ -1379,7 +1379,7 @@
         <v>27.14</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="12.75">
@@ -1387,7 +1387,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>16</v>
@@ -1412,7 +1412,7 @@
         <v>27.95</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="12.75">
@@ -1420,7 +1420,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>16</v>
@@ -1429,7 +1429,7 @@
         <v>30.08</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" s="17">
         <v>25.89</v>
@@ -1447,7 +1447,7 @@
         <v>30.97</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="12.75">
@@ -1455,7 +1455,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>21</v>
@@ -1464,7 +1464,7 @@
         <v>32.17</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" s="17">
         <v>23.34</v>
@@ -1482,7 +1482,7 @@
         <v>43.56</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="12.75">
@@ -1490,10 +1490,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="17">
         <v>34.15</v>
@@ -1515,7 +1515,7 @@
         <v>30.56</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="12.75">
@@ -1523,10 +1523,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="17">
         <f>(SUM(F20:J20)-MAX(F20:J20)-MIN(F20:J20))/3</f>
@@ -1549,10 +1549,10 @@
         <v>40.094999999999999</v>
       </c>
       <c r="K20" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="L20" s="22" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="12.75">
@@ -1560,7 +1560,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>21</v>
@@ -1569,7 +1569,7 @@
         <v>42.93</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="17">
         <v>35.76</v>
@@ -1587,7 +1587,7 @@
         <v>42.46</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="12.75">
@@ -1595,10 +1595,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="17">
         <v>44.11</v>
@@ -1620,7 +1620,7 @@
         <v>41.63</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="12.75">
@@ -1628,7 +1628,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>21</v>
@@ -1637,13 +1637,13 @@
         <v>50.72</v>
       </c>
       <c r="E23" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F23" s="17">
         <v>53.96</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H23" s="17">
         <v>44.3</v>
@@ -1655,7 +1655,7 @@
         <v>44.56</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="12.75">
@@ -1663,7 +1663,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>21</v>
@@ -1672,10 +1672,10 @@
         <v>60.84</v>
       </c>
       <c r="E24" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G24" s="17">
         <v>58.8</v>
@@ -1687,10 +1687,10 @@
         <v>58.48</v>
       </c>
       <c r="J24" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K24" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="12.75">
@@ -8742,8 +8742,8 @@
   </sheetPr>
   <dimension ref="A1:L1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8902,7 +8902,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>31</v>
@@ -8955,7 +8955,7 @@
         <v>45</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K7" s="18" t="s">
         <v>46</v>
@@ -8986,13 +8986,13 @@
         <v>53</v>
       </c>
       <c r="I8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K8" s="18" t="s">
         <v>54</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="L8" s="22"/>
     </row>
@@ -9001,32 +9001,32 @@
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="23"/>
       <c r="F9" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="H9" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K9" s="18" t="s">
         <v>61</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="12.75">
@@ -9034,32 +9034,32 @@
         <v>7</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="E10" s="23"/>
       <c r="F10" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="H10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="I10" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="12.75">
@@ -9067,32 +9067,32 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="23"/>
       <c r="F11" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G11" s="37" t="s">
-        <v>117</v>
-      </c>
       <c r="H11" s="37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12.75">
@@ -9100,32 +9100,32 @@
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="H12" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="I12" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K12" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12.75">
@@ -9133,35 +9133,35 @@
         <v>10</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="42" t="s">
-        <v>132</v>
-      </c>
       <c r="H13" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K13" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="I13" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="41" t="s">
-        <v>84</v>
-      </c>
       <c r="L13" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="12.75">
@@ -9169,32 +9169,32 @@
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G14" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" s="36" t="s">
-        <v>121</v>
-      </c>
       <c r="I14" s="17" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="K14" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12.75">
@@ -9202,32 +9202,32 @@
         <v>12</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="H15" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="I15" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="K15" s="41" t="s">
         <v>96</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="41" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="12.75">

</xml_diff>